<commit_message>
updated prolific proj id
</commit_message>
<xml_diff>
--- a/easyEyesSpreadsheets/CrowdingReadingAcuity.xlsx
+++ b/easyEyesSpreadsheets/CrowdingReadingAcuity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fh986/Documents/Github/crowding-individual-difference/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenhu/Documents/GitHub/crowding-individual-difference/easyEyesSpreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3D22D1-027F-834F-9013-2C168DBB1AAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58EF691-DFDF-844C-ADF3-441F9E74529F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="660" windowWidth="50900" windowHeight="26220" xr2:uid="{F1A85D42-BFAE-944F-85F3-75B22481207D}"/>
+    <workbookView xWindow="1100" yWindow="760" windowWidth="29140" windowHeight="18880" xr2:uid="{F1A85D42-BFAE-944F-85F3-75B22481207D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -581,9 +581,6 @@
 Click on PROCEED to continue.</t>
   </si>
   <si>
-    <t>624cbcd4c9f2ebe61823d39a</t>
-  </si>
-  <si>
     <t>Anna Bruns, Helen Hu, Jonathan Winawer, Denis Pelli</t>
   </si>
   <si>
@@ -711,6 +708,9 @@
   </si>
   <si>
     <t>crowding_R8_block4</t>
+  </si>
+  <si>
+    <t>67506ef48ae0fbccdc9b0326</t>
   </si>
 </sst>
 </file>
@@ -1207,10 +1207,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09F42C05-3A7A-B849-89F1-BA0E282F9675}">
   <dimension ref="A1:AG117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A31" sqref="A31"/>
-      <selection pane="topRight" activeCell="Y29" sqref="Y29"/>
+      <selection pane="topRight" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1224,7 +1224,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1232,7 +1232,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1375,8 +1375,8 @@
       <c r="A20" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>177</v>
+      <c r="B20" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.2">
@@ -1511,25 +1511,25 @@
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>214</v>
-      </c>
       <c r="D26" s="30" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F26" s="30" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G26" s="30" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H26" s="30" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>148</v>
@@ -1550,34 +1550,34 @@
         <v>148</v>
       </c>
       <c r="O26" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P26" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Q26" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="R26" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="S26" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="T26" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="U26" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="V26" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="W26" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="X26" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Y26" s="1" t="s">
         <v>149</v>
@@ -1598,13 +1598,13 @@
         <v>149</v>
       </c>
       <c r="AE26" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AF26" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AG26" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.2">
@@ -1826,91 +1826,91 @@
         <v>38</v>
       </c>
       <c r="C30" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="D30" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="E30" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="I30" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="E30" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F30" s="10" t="s">
+      <c r="J30" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="K30" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="G30" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="H30" s="10" t="s">
+      <c r="L30" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="M30" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="I30" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="J30" s="18" t="s">
+      <c r="N30" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="O30" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="K30" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="L30" s="18" t="s">
+      <c r="P30" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q30" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="M30" s="17" t="s">
-        <v>195</v>
-      </c>
-      <c r="N30" s="18" t="s">
+      <c r="R30" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="S30" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="O30" s="25" t="s">
-        <v>183</v>
-      </c>
-      <c r="P30" s="26" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q30" s="25" t="s">
-        <v>189</v>
-      </c>
-      <c r="R30" s="26" t="s">
-        <v>190</v>
-      </c>
-      <c r="S30" s="25" t="s">
+      <c r="T30" s="26" t="s">
         <v>197</v>
       </c>
-      <c r="T30" s="26" t="s">
-        <v>198</v>
-      </c>
       <c r="U30" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="V30" s="26" t="s">
         <v>217</v>
       </c>
-      <c r="V30" s="26" t="s">
+      <c r="W30" s="25" t="s">
         <v>218</v>
       </c>
-      <c r="W30" s="25" t="s">
+      <c r="X30" s="26" t="s">
         <v>219</v>
       </c>
-      <c r="X30" s="26" t="s">
-        <v>220</v>
-      </c>
       <c r="Y30" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="Z30" s="1"/>
       <c r="AA30" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AB30" s="1"/>
       <c r="AC30" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AD30" s="1"/>
       <c r="AE30" s="3" t="s">
         <v>39</v>
       </c>
       <c r="AF30" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AG30" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.2">
@@ -3935,7 +3935,7 @@
       <c r="X58" s="24"/>
       <c r="Y58" s="1"/>
       <c r="Z58" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AA58" s="1"/>
       <c r="AB58" s="1" t="s">
@@ -3977,7 +3977,7 @@
       <c r="X59" s="24"/>
       <c r="Y59" s="1"/>
       <c r="Z59" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AA59" s="1"/>
       <c r="AB59" s="1" t="s">
@@ -4019,7 +4019,7 @@
       <c r="X60" s="24"/>
       <c r="Y60" s="1"/>
       <c r="Z60" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AA60" s="1"/>
       <c r="AB60" s="1" t="s">
@@ -4061,7 +4061,7 @@
       <c r="X61" s="24"/>
       <c r="Y61" s="1"/>
       <c r="Z61" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AA61" s="1"/>
       <c r="AB61" s="1" t="s">
@@ -4103,7 +4103,7 @@
       <c r="X62" s="24"/>
       <c r="Y62" s="1"/>
       <c r="Z62" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AA62" s="1"/>
       <c r="AB62" s="1" t="s">
@@ -4144,15 +4144,15 @@
       <c r="W63" s="23"/>
       <c r="X63" s="24"/>
       <c r="Y63" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Z63" s="1"/>
       <c r="AA63" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AB63" s="1"/>
       <c r="AC63" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AD63" s="1"/>
       <c r="AE63" s="4" t="s">
@@ -4270,7 +4270,7 @@
       <c r="W66" s="23"/>
       <c r="X66" s="29"/>
       <c r="Y66" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Z66" s="1"/>
       <c r="AA66" s="1" t="s">
@@ -6779,7 +6779,7 @@
     </row>
     <row r="108" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C108" s="7">
         <v>1.4</v>

</xml_diff>